<commit_message>
Review and update docs.
</commit_message>
<xml_diff>
--- a/basedoc/ISR-catalog.xlsx
+++ b/basedoc/ISR-catalog.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$F$48</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$F$53</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="111">
   <si>
     <t xml:space="preserve">File</t>
   </si>
@@ -43,6 +43,27 @@
     <t xml:space="preserve">Remark</t>
   </si>
   <si>
+    <t xml:space="preserve">analog_comparator.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_ANALOG_COMPARE_ISR_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_ANALOG_COMPARE_ISR_METHOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CallbackHandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_ANALOG_COMPARE_ISR_EMPTY</t>
+  </si>
+  <si>
     <t xml:space="preserve">eeprom.h</t>
   </si>
   <si>
@@ -52,9 +73,6 @@
     <t xml:space="preserve">HandlerHolder</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">REGISTER_EEPROM_ISR_METHOD</t>
   </si>
   <si>
@@ -85,9 +103,6 @@
     <t xml:space="preserve">REGISTER_INT_ISR_EMPTY</t>
   </si>
   <si>
-    <t xml:space="preserve">NONE</t>
-  </si>
-  <si>
     <t xml:space="preserve">pci.h</t>
   </si>
   <si>
@@ -154,15 +169,30 @@
     <t xml:space="preserve">soft_uart.h</t>
   </si>
   <si>
+    <t xml:space="preserve">REGISTER_UARX_PCI_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler::check_uarx_pci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_UARX_INT_ISR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isr_handler::check_uarx_int</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGISTER_UART_PCI_ISR</t>
   </si>
   <si>
-    <t xml:space="preserve">isr_handler_check_pci_pins, HandlerHolder</t>
+    <t xml:space="preserve">isr_handler::check_uart_pci</t>
   </si>
   <si>
     <t xml:space="preserve">REGISTER_UART_INT_ISR</t>
   </si>
   <si>
+    <t xml:space="preserve">isr_handler::check_uart_int</t>
+  </si>
+  <si>
     <t xml:space="preserve">timer.h</t>
   </si>
   <si>
@@ -235,9 +265,6 @@
     <t xml:space="preserve">REGISTER_WATCHDOG_ISR_METHOD</t>
   </si>
   <si>
-    <t xml:space="preserve">CallbackHandler</t>
-  </si>
-  <si>
     <t xml:space="preserve">REGISTER_WATCHDOG_ISR_FUNCTION</t>
   </si>
   <si>
@@ -326,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">REGISTER_MULTI_HCSR04_RTT_TIMEOUT_FUNCTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTER_MULTI_HCSR04_RTT_TIMEOUT_TRIGGER_FUNCTION</t>
   </si>
 </sst>
 </file>
@@ -452,12 +482,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -471,18 +501,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ51"/>
+  <dimension ref="A1:AMJ57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="59.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.57"/>
@@ -528,9 +558,10 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="AMJ2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -542,13 +573,14 @@
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="AMJ3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
@@ -556,6 +588,7 @@
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="AMJ4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -568,128 +601,128 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,10 +736,10 @@
         <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,232 +747,232 @@
         <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>20</v>
+      <c r="C22" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D28" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,27 +983,24 @@
         <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,97 +1011,100 @@
         <v>8</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2" t="s">
-        <v>76</v>
+      <c r="B38" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,123 +1112,144 @@
         <v>80</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="D44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="9" t="s">
+      <c r="C45" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>89</v>
+      <c r="D45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>89</v>
+      <c r="C46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,11 +1257,71 @@
         <v>100</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F48"/>
+  <autoFilter ref="A1:F53"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>